<commit_message>
Working on: Front End Back End connections
</commit_message>
<xml_diff>
--- a/Credits/Sources-Creators.xlsx
+++ b/Credits/Sources-Creators.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
   <si>
     <t>Content</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>https://unsplash.com/photos/9vf1uj6i6Ww</t>
+  </si>
+  <si>
+    <t>Purple Swirl</t>
+  </si>
+  <si>
+    <t>Pawel Czerwinski</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/fPN1w7bIuNU</t>
   </si>
   <si>
     <t>Product Cards</t>
@@ -1109,7 +1118,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.10526315789474" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -1191,10 +1200,18 @@
       </c>
     </row>
     <row r="6" ht="16.8" spans="1:4">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" ht="16.8" spans="1:4">
       <c r="A7" s="7"/>
@@ -1407,6 +1424,7 @@
     <hyperlink ref="D4" r:id="rId3" display="https://unsplash.com/photos/DAoAtOXt1uY"/>
     <hyperlink ref="D3" r:id="rId4" display="https://unsplash.com/photos/p7WQxx8-xgM"/>
     <hyperlink ref="D5" r:id="rId5" display="https://unsplash.com/photos/9vf1uj6i6Ww"/>
+    <hyperlink ref="C6" r:id="rId6" display="Pawel Czerwinski" tooltip="https://unsplash.com/@pawel_czerwinski"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1446,16 +1464,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>